<commit_message>
Re-added the MockData.xlsx after accidental deletion
</commit_message>
<xml_diff>
--- a/Backend/data_processing/MockData.xlsx
+++ b/Backend/data_processing/MockData.xlsx
@@ -1,21 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navreetkaur/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7ED2828C-E8E5-7342-A55F-4D5910121202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D1639FB-0D04-0443-BA17-8717D235028F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -61,253 +77,253 @@
     <t>R001</t>
   </si>
   <si>
+    <t>10 Tui Road</t>
+  </si>
+  <si>
+    <t>Manurewa</t>
+  </si>
+  <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>Rent</t>
+  </si>
+  <si>
+    <t>Harcourts</t>
+  </si>
+  <si>
+    <t>Competitive market with similar listings</t>
+  </si>
+  <si>
     <t>R002</t>
   </si>
   <si>
+    <t>25A Mahia Road</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Ray White</t>
+  </si>
+  <si>
+    <t>Limited demand for smaller units in area</t>
+  </si>
+  <si>
     <t>R003</t>
   </si>
   <si>
+    <t>15B Great South Road</t>
+  </si>
+  <si>
+    <t>Papakura</t>
+  </si>
+  <si>
+    <t>Barfoot &amp; Thompson</t>
+  </si>
+  <si>
+    <t>Higher rent compared to similar properties</t>
+  </si>
+  <si>
     <t>R004</t>
   </si>
   <si>
+    <t>8 Karaka Street</t>
+  </si>
+  <si>
+    <t>Otara</t>
+  </si>
+  <si>
+    <t>LJ Hooker</t>
+  </si>
+  <si>
+    <t>Property requires maintenance</t>
+  </si>
+  <si>
     <t>R005</t>
   </si>
   <si>
+    <t>12 Mangere Road</t>
+  </si>
+  <si>
+    <t>Mangere</t>
+  </si>
+  <si>
+    <t>Apartment</t>
+  </si>
+  <si>
+    <t>Professionals</t>
+  </si>
+  <si>
+    <t>Recent listing</t>
+  </si>
+  <si>
     <t>R006</t>
   </si>
   <si>
+    <t>7 Hill Road</t>
+  </si>
+  <si>
+    <t>Manukau</t>
+  </si>
+  <si>
+    <t>Studio</t>
+  </si>
+  <si>
+    <t>City Rentals</t>
+  </si>
+  <si>
     <t>R007</t>
   </si>
   <si>
+    <t>18A Clevedon Road</t>
+  </si>
+  <si>
+    <t>Townhouse</t>
+  </si>
+  <si>
+    <t>Bayleys</t>
+  </si>
+  <si>
+    <t>Niche property type</t>
+  </si>
+  <si>
     <t>R008</t>
   </si>
   <si>
+    <t>22 Browns Road</t>
+  </si>
+  <si>
     <t>R009</t>
   </si>
   <si>
+    <t>5A Massey Road</t>
+  </si>
+  <si>
     <t>R010</t>
   </si>
   <si>
+    <t>3 Station Road</t>
+  </si>
+  <si>
     <t>R011</t>
   </si>
   <si>
+    <t>11 Tui Road</t>
+  </si>
+  <si>
     <t>R012</t>
   </si>
   <si>
+    <t>12 Mahia Road</t>
+  </si>
+  <si>
     <t>R013</t>
   </si>
   <si>
+    <t>13 Great South Road</t>
+  </si>
+  <si>
     <t>R014</t>
   </si>
   <si>
+    <t>14 Karaka Street</t>
+  </si>
+  <si>
     <t>R015</t>
   </si>
   <si>
+    <t>15 Mangere Road</t>
+  </si>
+  <si>
     <t>R016</t>
   </si>
   <si>
+    <t>16 Hill Road</t>
+  </si>
+  <si>
     <t>R017</t>
   </si>
   <si>
+    <t>17 Clevedon Road</t>
+  </si>
+  <si>
     <t>R018</t>
   </si>
   <si>
+    <t>18 Browns Road</t>
+  </si>
+  <si>
     <t>R019</t>
   </si>
   <si>
+    <t>19 Massey Road</t>
+  </si>
+  <si>
     <t>R020</t>
   </si>
   <si>
+    <t>20 Station Road</t>
+  </si>
+  <si>
     <t>R021</t>
   </si>
   <si>
+    <t>21 Tui Road</t>
+  </si>
+  <si>
     <t>R022</t>
   </si>
   <si>
+    <t>22 Mahia Road</t>
+  </si>
+  <si>
     <t>R023</t>
   </si>
   <si>
+    <t>23 Great South Road</t>
+  </si>
+  <si>
     <t>R024</t>
   </si>
   <si>
+    <t>24 Karaka Street</t>
+  </si>
+  <si>
     <t>R025</t>
   </si>
   <si>
+    <t>25 Mangere Road</t>
+  </si>
+  <si>
     <t>R026</t>
   </si>
   <si>
+    <t>26 Hill Road</t>
+  </si>
+  <si>
     <t>R027</t>
   </si>
   <si>
+    <t>27 Clevedon Road</t>
+  </si>
+  <si>
     <t>R028</t>
   </si>
   <si>
+    <t>28 Browns Road</t>
+  </si>
+  <si>
     <t>R029</t>
   </si>
   <si>
+    <t>29 Massey Road</t>
+  </si>
+  <si>
     <t>R030</t>
   </si>
   <si>
-    <t>10 Tui Road</t>
-  </si>
-  <si>
-    <t>25A Mahia Road</t>
-  </si>
-  <si>
-    <t>15B Great South Road</t>
-  </si>
-  <si>
-    <t>8 Karaka Street</t>
-  </si>
-  <si>
-    <t>12 Mangere Road</t>
-  </si>
-  <si>
-    <t>7 Hill Road</t>
-  </si>
-  <si>
-    <t>18A Clevedon Road</t>
-  </si>
-  <si>
-    <t>22 Browns Road</t>
-  </si>
-  <si>
-    <t>5A Massey Road</t>
-  </si>
-  <si>
-    <t>3 Station Road</t>
-  </si>
-  <si>
-    <t>11 Tui Road</t>
-  </si>
-  <si>
-    <t>12 Mahia Road</t>
-  </si>
-  <si>
-    <t>13 Great South Road</t>
-  </si>
-  <si>
-    <t>14 Karaka Street</t>
-  </si>
-  <si>
-    <t>15 Mangere Road</t>
-  </si>
-  <si>
-    <t>16 Hill Road</t>
-  </si>
-  <si>
-    <t>17 Clevedon Road</t>
-  </si>
-  <si>
-    <t>18 Browns Road</t>
-  </si>
-  <si>
-    <t>19 Massey Road</t>
-  </si>
-  <si>
-    <t>20 Station Road</t>
-  </si>
-  <si>
-    <t>21 Tui Road</t>
-  </si>
-  <si>
-    <t>22 Mahia Road</t>
-  </si>
-  <si>
-    <t>23 Great South Road</t>
-  </si>
-  <si>
-    <t>24 Karaka Street</t>
-  </si>
-  <si>
-    <t>25 Mangere Road</t>
-  </si>
-  <si>
-    <t>26 Hill Road</t>
-  </si>
-  <si>
-    <t>27 Clevedon Road</t>
-  </si>
-  <si>
-    <t>28 Browns Road</t>
-  </si>
-  <si>
-    <t>29 Massey Road</t>
-  </si>
-  <si>
     <t>30 Station Road</t>
-  </si>
-  <si>
-    <t>Manurewa</t>
-  </si>
-  <si>
-    <t>Papakura</t>
-  </si>
-  <si>
-    <t>Otara</t>
-  </si>
-  <si>
-    <t>Mangere</t>
-  </si>
-  <si>
-    <t>Manukau</t>
-  </si>
-  <si>
-    <t>House</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>Apartment</t>
-  </si>
-  <si>
-    <t>Studio</t>
-  </si>
-  <si>
-    <t>Townhouse</t>
-  </si>
-  <si>
-    <t>Rent</t>
-  </si>
-  <si>
-    <t>Harcourts</t>
-  </si>
-  <si>
-    <t>Ray White</t>
-  </si>
-  <si>
-    <t>Barfoot &amp; Thompson</t>
-  </si>
-  <si>
-    <t>LJ Hooker</t>
-  </si>
-  <si>
-    <t>Professionals</t>
-  </si>
-  <si>
-    <t>City Rentals</t>
-  </si>
-  <si>
-    <t>Bayleys</t>
-  </si>
-  <si>
-    <t>Competitive market with similar listings</t>
-  </si>
-  <si>
-    <t>Limited demand for smaller units in area</t>
-  </si>
-  <si>
-    <t>Higher rent compared to similar properties</t>
-  </si>
-  <si>
-    <t>Property requires maintenance</t>
-  </si>
-  <si>
-    <t>Recent listing</t>
-  </si>
-  <si>
-    <t>Niche property type</t>
   </si>
 </sst>
 </file>
@@ -677,7 +693,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -736,10 +754,10 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>3</v>
@@ -748,7 +766,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G2">
         <v>550</v>
@@ -757,27 +775,27 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J2">
         <v>12</v>
       </c>
       <c r="K2" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="L2" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -786,7 +804,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="G3">
         <v>480</v>
@@ -795,27 +813,27 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J3">
         <v>8</v>
       </c>
       <c r="K3" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="L3" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="D4">
         <v>4</v>
@@ -824,7 +842,7 @@
         <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G4">
         <v>620</v>
@@ -833,27 +851,27 @@
         <v>2</v>
       </c>
       <c r="I4" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J4">
         <v>15</v>
       </c>
       <c r="K4" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="L4" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="D5">
         <v>3</v>
@@ -862,7 +880,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G5">
         <v>510</v>
@@ -871,27 +889,27 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J5">
         <v>20</v>
       </c>
       <c r="K5" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="L5" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -900,7 +918,7 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="G6">
         <v>470</v>
@@ -909,27 +927,27 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J6">
         <v>5</v>
       </c>
       <c r="K6" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="L6" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="D7">
         <v>1</v>
@@ -938,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="G7">
         <v>400</v>
@@ -947,27 +965,27 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J7">
         <v>3</v>
       </c>
       <c r="K7" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="L7" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -976,7 +994,7 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="G8">
         <v>580</v>
@@ -985,27 +1003,27 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J8">
         <v>10</v>
       </c>
       <c r="K8" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="L8" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="D9">
         <v>4</v>
@@ -1014,7 +1032,7 @@
         <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G9">
         <v>630</v>
@@ -1023,27 +1041,27 @@
         <v>2</v>
       </c>
       <c r="I9" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J9">
         <v>7</v>
       </c>
       <c r="K9" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="L9" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -1052,7 +1070,7 @@
         <v>1</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="G10">
         <v>460</v>
@@ -1061,27 +1079,27 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J10">
         <v>14</v>
       </c>
       <c r="K10" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="L10" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>54</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -1090,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G11">
         <v>520</v>
@@ -1099,27 +1117,27 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J11">
         <v>9</v>
       </c>
       <c r="K11" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="L11" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="D12">
         <v>3</v>
@@ -1128,7 +1146,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G12">
         <v>570</v>
@@ -1137,27 +1155,27 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J12">
         <v>13</v>
       </c>
       <c r="K12" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="L12" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="D13">
         <v>2</v>
@@ -1166,7 +1184,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="G13">
         <v>480</v>
@@ -1175,27 +1193,27 @@
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J13">
         <v>10</v>
       </c>
       <c r="K13" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="L13" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="D14">
         <v>4</v>
@@ -1204,7 +1222,7 @@
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G14">
         <v>630</v>
@@ -1213,27 +1231,27 @@
         <v>2</v>
       </c>
       <c r="I14" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J14">
         <v>18</v>
       </c>
       <c r="K14" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="L14" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>62</v>
       </c>
       <c r="B15" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <v>3</v>
@@ -1242,7 +1260,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G15">
         <v>530</v>
@@ -1251,27 +1269,27 @@
         <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J15">
         <v>24</v>
       </c>
       <c r="K15" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="L15" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1280,7 +1298,7 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="G16">
         <v>470</v>
@@ -1289,27 +1307,27 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J16">
         <v>5</v>
       </c>
       <c r="K16" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="L16" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="D17">
         <v>1</v>
@@ -1318,7 +1336,7 @@
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="G17">
         <v>410</v>
@@ -1327,27 +1345,27 @@
         <v>0</v>
       </c>
       <c r="I17" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J17">
         <v>4</v>
       </c>
       <c r="K17" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="L17" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>28</v>
+        <v>68</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -1356,7 +1374,7 @@
         <v>2</v>
       </c>
       <c r="F18" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="G18">
         <v>600</v>
@@ -1365,27 +1383,27 @@
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J18">
         <v>12</v>
       </c>
       <c r="K18" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="L18" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="D19">
         <v>4</v>
@@ -1394,7 +1412,7 @@
         <v>2</v>
       </c>
       <c r="F19" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G19">
         <v>630</v>
@@ -1403,27 +1421,27 @@
         <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J19">
         <v>10</v>
       </c>
       <c r="K19" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="L19" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="D20">
         <v>2</v>
@@ -1432,7 +1450,7 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="G20">
         <v>470</v>
@@ -1441,27 +1459,27 @@
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J20">
         <v>18</v>
       </c>
       <c r="K20" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="L20" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C21" t="s">
         <v>31</v>
-      </c>
-      <c r="B21" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" t="s">
-        <v>74</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -1470,7 +1488,7 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G21">
         <v>540</v>
@@ -1479,27 +1497,27 @@
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J21">
         <v>9</v>
       </c>
       <c r="K21" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="L21" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="C22" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="D22">
         <v>3</v>
@@ -1508,7 +1526,7 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G22">
         <v>550</v>
@@ -1517,27 +1535,27 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J22">
         <v>13</v>
       </c>
       <c r="K22" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="L22" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="C23" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="D23">
         <v>2</v>
@@ -1546,7 +1564,7 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="G23">
         <v>490</v>
@@ -1555,27 +1573,27 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J23">
         <v>10</v>
       </c>
       <c r="K23" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="L23" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>80</v>
       </c>
       <c r="B24" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="D24">
         <v>4</v>
@@ -1584,7 +1602,7 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G24">
         <v>640</v>
@@ -1593,27 +1611,27 @@
         <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J24">
         <v>18</v>
       </c>
       <c r="K24" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="L24" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>82</v>
       </c>
       <c r="B25" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="D25">
         <v>3</v>
@@ -1622,7 +1640,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G25">
         <v>510</v>
@@ -1631,28 +1649,28 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J25">
         <v>24</v>
       </c>
       <c r="K25" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
       <c r="L25" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>84</v>
+      </c>
+      <c r="B26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" t="s">
         <v>36</v>
       </c>
-      <c r="B26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" t="s">
-        <v>75</v>
-      </c>
       <c r="D26">
         <v>2</v>
       </c>
@@ -1660,7 +1678,7 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
-        <v>79</v>
+        <v>37</v>
       </c>
       <c r="G26">
         <v>480</v>
@@ -1669,27 +1687,27 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J26">
         <v>5</v>
       </c>
       <c r="K26" t="s">
-        <v>87</v>
+        <v>38</v>
       </c>
       <c r="L26" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="B27" t="s">
-        <v>67</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="D27">
         <v>1</v>
@@ -1698,7 +1716,7 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>80</v>
+        <v>43</v>
       </c>
       <c r="G27">
         <v>420</v>
@@ -1707,27 +1725,27 @@
         <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J27">
         <v>4</v>
       </c>
       <c r="K27" t="s">
-        <v>88</v>
+        <v>44</v>
       </c>
       <c r="L27" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="B28" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="D28">
         <v>3</v>
@@ -1736,7 +1754,7 @@
         <v>2</v>
       </c>
       <c r="F28" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="G28">
         <v>580</v>
@@ -1745,27 +1763,27 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J28">
         <v>12</v>
       </c>
       <c r="K28" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="L28" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>90</v>
       </c>
       <c r="B29" t="s">
-        <v>69</v>
+        <v>91</v>
       </c>
       <c r="C29" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="D29">
         <v>4</v>
@@ -1774,7 +1792,7 @@
         <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G29">
         <v>640</v>
@@ -1783,27 +1801,27 @@
         <v>2</v>
       </c>
       <c r="I29" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J29">
         <v>10</v>
       </c>
       <c r="K29" t="s">
-        <v>83</v>
+        <v>17</v>
       </c>
       <c r="L29" t="s">
-        <v>94</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>40</v>
+        <v>92</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>93</v>
       </c>
       <c r="C30" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -1812,7 +1830,7 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="G30">
         <v>480</v>
@@ -1821,27 +1839,27 @@
         <v>1</v>
       </c>
       <c r="I30" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J30">
         <v>18</v>
       </c>
       <c r="K30" t="s">
-        <v>84</v>
+        <v>22</v>
       </c>
       <c r="L30" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
       <c r="C31" t="s">
-        <v>74</v>
+        <v>31</v>
       </c>
       <c r="D31">
         <v>3</v>
@@ -1850,7 +1868,7 @@
         <v>1</v>
       </c>
       <c r="F31" t="s">
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="G31">
         <v>520</v>
@@ -1859,16 +1877,16 @@
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>82</v>
+        <v>16</v>
       </c>
       <c r="J31">
         <v>9</v>
       </c>
       <c r="K31" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="L31" t="s">
-        <v>90</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement model retraining with new data upload endpoint
</commit_message>
<xml_diff>
--- a/Backend/data_processing/MockData.xlsx
+++ b/Backend/data_processing/MockData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navreetkaur/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/dba924227dd0bfa8/Documents/GitHub/Mj-Homes-Dashboard/Backend/data_processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D1639FB-0D04-0443-BA17-8717D235028F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6535A6EC-E51F-4061-B62E-AB10A24DAD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -694,24 +694,24 @@
   <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="13.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" customWidth="1"/>
-    <col min="11" max="11" width="24.33203125" customWidth="1"/>
-    <col min="12" max="12" width="44.5" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="6" max="6" width="21.6328125" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="8" max="8" width="13.36328125" customWidth="1"/>
+    <col min="9" max="9" width="14.81640625" customWidth="1"/>
+    <col min="10" max="10" width="18.6328125" customWidth="1"/>
+    <col min="11" max="11" width="24.36328125" customWidth="1"/>
+    <col min="12" max="12" width="44.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -749,7 +749,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -787,7 +787,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -825,7 +825,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -863,7 +863,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -901,7 +901,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -939,7 +939,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -977,7 +977,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1015,7 +1015,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>52</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -1129,7 +1129,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>58</v>
       </c>
@@ -1205,7 +1205,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>60</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>62</v>
       </c>
@@ -1281,7 +1281,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>64</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -1357,7 +1357,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>70</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -1471,7 +1471,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>76</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>78</v>
       </c>
@@ -1585,7 +1585,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>80</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>82</v>
       </c>
@@ -1661,7 +1661,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>86</v>
       </c>
@@ -1737,7 +1737,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>88</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>90</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>92</v>
       </c>
@@ -1851,7 +1851,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>94</v>
       </c>

</xml_diff>